<commit_message>
New Feature added to tool it has the ability to run a high volume of test cases and automatically generate log reports which show the results in an easy-to-read format.
</commit_message>
<xml_diff>
--- a/BatchExecution_BI/src/ConfigFiles/Config.xlsx
+++ b/BatchExecution_BI/src/ConfigFiles/Config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>Teradata_Username</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Run</t>
+  </si>
+  <si>
+    <t>O64QoSDUFWyJJSpQl9fUJg==</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>

</xml_diff>